<commit_message>
finalisation du model de planning
ajout des dates
</commit_message>
<xml_diff>
--- a/Documentation/HoferL-Journal&Planif-M5.xlsx
+++ b/Documentation/HoferL-Journal&Planif-M5.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Graphique" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="PlanificationExemple" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="SommeParJours" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="Plannification" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PlanificationExemple" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="SommeParJours" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$B$2:$H$30</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>date</t>
   </si>
@@ -108,12 +109,117 @@
     <t>Somme</t>
   </si>
   <si>
+    <t>Janvier</t>
+  </si>
+  <si>
+    <t>Février</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Avril</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Juin</t>
+  </si>
+  <si>
     <t>Phases</t>
   </si>
   <si>
     <t>Tâche</t>
   </si>
   <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>26.01.2026</t>
+  </si>
+  <si>
+    <t>02.02.2026</t>
+  </si>
+  <si>
+    <t>09.03.2026</t>
+  </si>
+  <si>
+    <t>10.03.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacances (16-20 fev.)</t>
+  </si>
+  <si>
+    <t>23.02.2026</t>
+  </si>
+  <si>
+    <t>24.02.2026</t>
+  </si>
+  <si>
+    <t>02.03.2026</t>
+  </si>
+  <si>
+    <t>03.03.2026</t>
+  </si>
+  <si>
+    <t>16.03.2026</t>
+  </si>
+  <si>
+    <t>17.03.2026</t>
+  </si>
+  <si>
+    <t>24.03.2026</t>
+  </si>
+  <si>
+    <t>30.03.2026</t>
+  </si>
+  <si>
+    <t>31.03.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vacances (6-18 avr.)</t>
+  </si>
+  <si>
+    <t>20.04.2026</t>
+  </si>
+  <si>
+    <t>21.04.2026</t>
+  </si>
+  <si>
+    <t>28.04.2026</t>
+  </si>
+  <si>
+    <t>04.05.2026</t>
+  </si>
+  <si>
+    <t>05.05.2026</t>
+  </si>
+  <si>
+    <t>12.05.2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absent (18-22 Mai)</t>
+  </si>
+  <si>
+    <t>26.05.2026</t>
+  </si>
+  <si>
+    <t>01.06.2026</t>
+  </si>
+  <si>
+    <t>02.06.2026</t>
+  </si>
+  <si>
+    <t>08.06.2026</t>
+  </si>
+  <si>
+    <t>09.06.2026</t>
+  </si>
+  <si>
+    <t>11.06.2026</t>
+  </si>
+  <si>
     <t>Mois</t>
   </si>
   <si>
@@ -124,12 +230,6 @@
   </si>
   <si>
     <t>Décembre</t>
-  </si>
-  <si>
-    <t>Janvier</t>
-  </si>
-  <si>
-    <t>Février</t>
   </si>
   <si>
     <t>S</t>
@@ -229,10 +329,16 @@
     <numFmt numFmtId="168" formatCode="d/m/yy;@"/>
     <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -305,6 +411,37 @@
     <border>
       <left style="none"/>
       <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
       <top style="medium">
         <color auto="1"/>
       </top>
@@ -359,17 +496,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="none"/>
-      <bottom style="none"/>
       <diagonal style="none"/>
     </border>
     <border>
@@ -602,15 +728,6 @@
     </border>
     <border>
       <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
-    <border>
-      <left style="none"/>
       <right style="mediumDashed">
         <color auto="1"/>
       </right>
@@ -1019,22 +1136,11 @@
       </bottom>
       <diagonal style="none"/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="none"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="136">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1079,40 +1185,92 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="15" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="180" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="180" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="180" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="15" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="0" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1120,126 +1278,129 @@
     <xf fontId="0" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="13" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="20" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="19" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="22" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="22" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="21" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="22" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="23" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="24" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="24" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="25" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="26" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="25" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="28" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="27" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="29" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="30" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="29" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="28" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="30" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="30" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="31" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="32" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="32" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="33" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="33" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="13" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="23" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="18" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="24" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="31" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="5" borderId="19" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="20" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="26" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="32" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="5" borderId="21" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="35" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="36" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="37" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="37" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="38" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="38" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="39" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="39" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="40" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="40" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="41" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="42" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="43" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="43" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="18" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="44" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="44" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="45" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="45" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="46" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="47" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="48" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="46" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="49" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="50" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="47" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="50" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="51" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="52" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="27" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="47" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="53" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="29" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="4" borderId="48" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="53" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="49" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="54" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="55" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="56" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="12" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="57" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="57" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="58" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="58" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="59" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="59" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="60" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="60" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="61" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="62" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="63" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="64" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="64" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="34" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="33" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="168" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="169" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -5878,7 +6039,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1" disablePrompts="0">
-        <x14:dataValidation xr:uid="{006A0002-00D7-4D1B-BA87-00C0005A0031}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{0060003B-00C6-4B37-A119-005200D8001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>$G$3:$G$7</xm:f>
           </x14:formula1>
@@ -5918,6 +6079,227 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="3" max="3" width="31.29296875"/>
+    <col customWidth="1" min="5" max="49" width="3.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30.5" customHeight="1">
+      <c r="E1" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+    </row>
+    <row r="2" ht="98.5" customHeight="1">
+      <c r="B2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="X2" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE2" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="AG2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI2" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ2" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK2" s="29"/>
+      <c r="AL2" s="29"/>
+      <c r="AM2" s="29"/>
+      <c r="AN2" s="29"/>
+      <c r="AO2" s="29"/>
+      <c r="AP2" s="29"/>
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="29"/>
+      <c r="AS2" s="29"/>
+      <c r="AT2" s="29"/>
+      <c r="AU2" s="29"/>
+      <c r="AV2" s="29"/>
+      <c r="AW2" s="29"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+    </row>
+    <row r="55" ht="14.25">
+      <c r="C55" s="30"/>
+      <c r="D55" s="31"/>
+    </row>
+    <row r="56" ht="14.25">
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
+    </row>
+    <row r="57" ht="14.25">
+      <c r="C57" s="32"/>
+      <c r="D57" s="34"/>
+    </row>
+    <row r="58" ht="14.25">
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:N1"/>
+    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
     <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
@@ -5942,801 +6324,801 @@
   </cols>
   <sheetData>
     <row r="1" ht="15">
-      <c r="B1" s="16"/>
+      <c r="B1" s="35"/>
     </row>
     <row r="2" ht="56.399999999999999" customHeight="1">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="22"/>
-      <c r="AD2" s="23"/>
+      <c r="S2" s="41"/>
+      <c r="AD2" s="42"/>
     </row>
     <row r="3" ht="15">
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" s="27">
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="46">
         <v>4</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="47">
         <v>1</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="48">
         <v>2</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="48">
         <v>3</v>
       </c>
-      <c r="I3" s="27">
+      <c r="I3" s="46">
         <v>4</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="47">
         <v>1</v>
       </c>
-      <c r="K3" s="29">
+      <c r="K3" s="48">
         <v>2</v>
       </c>
-      <c r="L3" s="29">
+      <c r="L3" s="48">
         <v>3</v>
       </c>
-      <c r="M3" s="27">
+      <c r="M3" s="46">
         <v>4</v>
       </c>
-      <c r="N3" s="28">
+      <c r="N3" s="47">
         <v>1</v>
       </c>
-      <c r="O3" s="29">
+      <c r="O3" s="48">
         <v>2</v>
       </c>
-      <c r="P3" s="29">
+      <c r="P3" s="48">
         <v>3</v>
       </c>
-      <c r="Q3" s="27">
+      <c r="Q3" s="46">
         <v>4</v>
       </c>
-      <c r="R3" s="28">
+      <c r="R3" s="47">
         <v>1</v>
       </c>
-      <c r="S3" s="30">
+      <c r="S3" s="49">
         <v>2</v>
       </c>
       <c r="U3" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" ht="12" customHeight="1">
-      <c r="B4" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="37"/>
+      <c r="B4" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="51"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="55"/>
+      <c r="S4" s="56"/>
       <c r="U4" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" ht="12" customHeight="1">
-      <c r="B5" s="31"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="43"/>
-      <c r="L5" s="43"/>
-      <c r="M5" s="40"/>
-      <c r="N5" s="44"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="43"/>
-      <c r="Q5" s="40"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="45"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="64"/>
     </row>
     <row r="6" ht="12" customHeight="1">
-      <c r="B6" s="31"/>
-      <c r="C6" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="47"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="51"/>
-      <c r="L6" s="51"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="51"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="53"/>
-      <c r="U6" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="V6" s="54"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="71"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="67"/>
+      <c r="R6" s="71"/>
+      <c r="S6" s="72"/>
+      <c r="U6" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="V6" s="73"/>
     </row>
     <row r="7" ht="12" customHeight="1">
-      <c r="B7" s="31"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="40"/>
-      <c r="N7" s="44"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="40"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="45"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="64"/>
       <c r="U7" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" ht="12" customHeight="1">
-      <c r="B8" s="31"/>
-      <c r="C8" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="52"/>
-      <c r="S8" s="53"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="66"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="72"/>
       <c r="U8" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" ht="12" customHeight="1">
-      <c r="B9" s="31"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="43"/>
-      <c r="L9" s="43"/>
-      <c r="M9" s="40"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="43"/>
-      <c r="P9" s="43"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="45"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="64"/>
     </row>
     <row r="10" ht="12" customHeight="1">
-      <c r="B10" s="31"/>
-      <c r="C10" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="47"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="52"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="52"/>
-      <c r="S10" s="53"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="72"/>
     </row>
     <row r="11" ht="12" customHeight="1">
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="58"/>
-      <c r="R11" s="59"/>
-      <c r="S11" s="62"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="77"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="80"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="78"/>
+      <c r="S11" s="81"/>
     </row>
     <row r="12" ht="12" customHeight="1">
-      <c r="B12" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="37"/>
+      <c r="B12" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="51"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="55"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="56"/>
     </row>
     <row r="13" ht="12" customHeight="1">
-      <c r="B13" s="31"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="40"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="40"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="45"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="64"/>
     </row>
     <row r="14" ht="12" customHeight="1">
-      <c r="B14" s="31"/>
-      <c r="C14" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="65"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="51"/>
-      <c r="P14" s="51"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="53"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="84"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="71"/>
+      <c r="O14" s="70"/>
+      <c r="P14" s="70"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="71"/>
+      <c r="S14" s="72"/>
     </row>
     <row r="15" ht="12" customHeight="1">
-      <c r="B15" s="31"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="44"/>
-      <c r="O15" s="43"/>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="45"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="64"/>
     </row>
     <row r="16" ht="12" customHeight="1">
-      <c r="B16" s="31"/>
-      <c r="C16" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="52"/>
-      <c r="S16" s="53"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="71"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="72"/>
     </row>
     <row r="17" ht="12" customHeight="1">
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="62"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="87"/>
+      <c r="K17" s="79"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="78"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="80"/>
+      <c r="Q17" s="77"/>
+      <c r="R17" s="78"/>
+      <c r="S17" s="81"/>
     </row>
     <row r="18" ht="12" customHeight="1">
-      <c r="B18" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="37"/>
+      <c r="B18" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="51"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="55"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="56"/>
     </row>
     <row r="19" ht="12" customHeight="1">
-      <c r="B19" s="31"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="40"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="45"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="62"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="59"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="64"/>
     </row>
     <row r="20" ht="12" customHeight="1">
-      <c r="B20" s="31"/>
-      <c r="C20" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="51"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="50"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="52"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="48"/>
-      <c r="R20" s="52"/>
-      <c r="S20" s="53"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="71"/>
+      <c r="O20" s="70"/>
+      <c r="P20" s="70"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="71"/>
+      <c r="S20" s="72"/>
     </row>
     <row r="21" ht="12" customHeight="1">
-      <c r="B21" s="31"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="43"/>
-      <c r="L21" s="43"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="43"/>
-      <c r="P21" s="43"/>
-      <c r="Q21" s="40"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="45"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="62"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="62"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="64"/>
     </row>
     <row r="22" ht="12" customHeight="1">
-      <c r="B22" s="31"/>
-      <c r="C22" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="50"/>
-      <c r="M22" s="48"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="48"/>
-      <c r="R22" s="52"/>
-      <c r="S22" s="53"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="65" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="66"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="71"/>
+      <c r="O22" s="70"/>
+      <c r="P22" s="70"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="71"/>
+      <c r="S22" s="72"/>
     </row>
     <row r="23" ht="12" customHeight="1">
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="62"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="80"/>
+      <c r="M23" s="77"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="80"/>
+      <c r="P23" s="80"/>
+      <c r="Q23" s="77"/>
+      <c r="R23" s="78"/>
+      <c r="S23" s="81"/>
     </row>
     <row r="24" ht="12" customHeight="1">
-      <c r="B24" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="63"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="37"/>
+      <c r="B24" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="54"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="83"/>
+      <c r="N24" s="53"/>
+      <c r="O24" s="82"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
     </row>
     <row r="25" ht="12" customHeight="1">
-      <c r="B25" s="31"/>
-      <c r="C25" s="38"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
-      <c r="M25" s="40"/>
-      <c r="N25" s="44"/>
-      <c r="O25" s="43"/>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="40"/>
-      <c r="R25" s="44"/>
-      <c r="S25" s="45"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="63"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="62"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="64"/>
     </row>
     <row r="26" ht="12" customHeight="1">
-      <c r="B26" s="31"/>
-      <c r="C26" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="52"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="48"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="48"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="50"/>
-      <c r="P26" s="50"/>
-      <c r="Q26" s="48"/>
-      <c r="R26" s="52"/>
-      <c r="S26" s="53"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="66"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="70"/>
+      <c r="L26" s="70"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="72"/>
     </row>
     <row r="27" ht="12" customHeight="1">
-      <c r="B27" s="31"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="43"/>
-      <c r="L27" s="43"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="44"/>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="40"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="45"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="64"/>
     </row>
     <row r="28" ht="12" customHeight="1">
-      <c r="B28" s="31"/>
-      <c r="C28" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="52"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="51"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="67"/>
-      <c r="R28" s="52"/>
-      <c r="S28" s="53"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="65" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="66"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="70"/>
+      <c r="P28" s="69"/>
+      <c r="Q28" s="86"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="72"/>
     </row>
     <row r="29" ht="12" customHeight="1">
-      <c r="B29" s="31"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="73"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="71"/>
-      <c r="J29" s="72"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="71"/>
-      <c r="N29" s="75"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="71"/>
-      <c r="R29" s="72"/>
-      <c r="S29" s="76"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="89"/>
+      <c r="E29" s="90"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="91"/>
+      <c r="K29" s="92"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="93"/>
+      <c r="P29" s="92"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="91"/>
+      <c r="S29" s="95"/>
     </row>
     <row r="30" ht="12" customHeight="1">
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="80"/>
-      <c r="H30" s="81"/>
-      <c r="I30" s="82"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="80"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="82"/>
-      <c r="N30" s="80"/>
-      <c r="O30" s="81"/>
-      <c r="P30" s="80"/>
-      <c r="Q30" s="82"/>
-      <c r="R30" s="80"/>
-      <c r="S30" s="83"/>
+      <c r="C30" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="51"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="99"/>
+      <c r="G30" s="99"/>
+      <c r="H30" s="100"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="99"/>
+      <c r="L30" s="100"/>
+      <c r="M30" s="101"/>
+      <c r="N30" s="99"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="99"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="102"/>
     </row>
     <row r="31" ht="12" customHeight="1">
-      <c r="B31" s="84"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="88"/>
-      <c r="I31" s="89"/>
-      <c r="J31" s="87"/>
-      <c r="K31" s="90"/>
-      <c r="L31" s="88"/>
-      <c r="M31" s="89"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="88"/>
-      <c r="P31" s="87"/>
-      <c r="Q31" s="89"/>
-      <c r="R31" s="87"/>
-      <c r="S31" s="45"/>
+      <c r="B31" s="103"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="105"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="107"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="106"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="108"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="106"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="106"/>
+      <c r="S31" s="64"/>
     </row>
     <row r="32" ht="12" customHeight="1">
-      <c r="B32" s="84"/>
-      <c r="C32" s="85" t="s">
+      <c r="B32" s="103"/>
+      <c r="C32" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="91"/>
-      <c r="F32" s="92"/>
-      <c r="G32" s="92"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="94"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="92"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="94"/>
-      <c r="N32" s="92"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="92"/>
-      <c r="Q32" s="94"/>
-      <c r="R32" s="92"/>
-      <c r="S32" s="95"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="111"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="113"/>
+      <c r="J32" s="111"/>
+      <c r="K32" s="111"/>
+      <c r="L32" s="112"/>
+      <c r="M32" s="113"/>
+      <c r="N32" s="111"/>
+      <c r="O32" s="112"/>
+      <c r="P32" s="111"/>
+      <c r="Q32" s="113"/>
+      <c r="R32" s="111"/>
+      <c r="S32" s="114"/>
     </row>
     <row r="33" ht="12" customHeight="1">
-      <c r="B33" s="84"/>
-      <c r="C33" s="85"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="86"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="96"/>
-      <c r="I33" s="97"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="88"/>
-      <c r="M33" s="89"/>
-      <c r="N33" s="87"/>
-      <c r="O33" s="88"/>
-      <c r="P33" s="87"/>
-      <c r="Q33" s="89"/>
-      <c r="R33" s="87"/>
-      <c r="S33" s="45"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="105"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="106"/>
+      <c r="H33" s="115"/>
+      <c r="I33" s="116"/>
+      <c r="J33" s="106"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="106"/>
+      <c r="O33" s="107"/>
+      <c r="P33" s="106"/>
+      <c r="Q33" s="108"/>
+      <c r="R33" s="106"/>
+      <c r="S33" s="64"/>
     </row>
     <row r="34" ht="12" customHeight="1">
-      <c r="B34" s="84"/>
-      <c r="C34" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="70"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="99"/>
-      <c r="K34" s="99"/>
-      <c r="L34" s="100"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="99"/>
-      <c r="O34" s="100"/>
-      <c r="P34" s="99"/>
-      <c r="Q34" s="101"/>
-      <c r="R34" s="99"/>
-      <c r="S34" s="102"/>
-      <c r="U34" s="103"/>
-      <c r="V34" s="104" t="s">
-        <v>61</v>
+      <c r="B34" s="103"/>
+      <c r="C34" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="89"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="118"/>
+      <c r="G34" s="118"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="118"/>
+      <c r="K34" s="118"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="120"/>
+      <c r="N34" s="118"/>
+      <c r="O34" s="119"/>
+      <c r="P34" s="118"/>
+      <c r="Q34" s="120"/>
+      <c r="R34" s="118"/>
+      <c r="S34" s="121"/>
+      <c r="U34" s="122"/>
+      <c r="V34" s="123" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="35" ht="13.800000000000001" customHeight="1">
-      <c r="B35" s="105"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="109"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="109"/>
-      <c r="M35" s="110"/>
-      <c r="N35" s="108"/>
-      <c r="O35" s="109"/>
-      <c r="P35" s="108"/>
-      <c r="Q35" s="110"/>
-      <c r="R35" s="108"/>
-      <c r="S35" s="62"/>
-      <c r="U35" s="111"/>
-      <c r="V35" s="112" t="s">
-        <v>62</v>
+      <c r="B35" s="124"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="126"/>
+      <c r="F35" s="127"/>
+      <c r="G35" s="127"/>
+      <c r="H35" s="128"/>
+      <c r="I35" s="129"/>
+      <c r="J35" s="127"/>
+      <c r="K35" s="127"/>
+      <c r="L35" s="128"/>
+      <c r="M35" s="129"/>
+      <c r="N35" s="127"/>
+      <c r="O35" s="128"/>
+      <c r="P35" s="127"/>
+      <c r="Q35" s="129"/>
+      <c r="R35" s="127"/>
+      <c r="S35" s="81"/>
+      <c r="U35" s="34"/>
+      <c r="V35" s="130" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -6777,7 +7159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
@@ -6786,7 +7168,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" style="113" width="11.5546875"/>
+    <col min="3" max="3" style="131" width="11.5546875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6796,1810 +7178,1810 @@
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="113" t="s">
-        <v>63</v>
+      <c r="C1" s="131" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="114">
+      <c r="A2" s="132">
         <f t="array" ref="A2:A11">_xlfn.UNIQUE(Journal[date])</f>
         <v>45958</v>
       </c>
-      <c r="B2" s="115">
+      <c r="B2" s="133">
         <f t="shared" ref="B2:B65" si="0">IF(C2&gt;0,C2,"")</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C2" s="116">
+      <c r="C2" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A2,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="114">
+      <c r="A3" s="132">
         <f/>
         <v>45965</v>
       </c>
-      <c r="B3" s="115">
+      <c r="B3" s="133">
         <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
-      <c r="C3" s="116">
+      <c r="C3" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A3,Journal[Temps])</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="114">
+      <c r="A4" s="132">
         <f/>
         <v>45972</v>
       </c>
-      <c r="B4" s="115">
+      <c r="B4" s="133">
         <f t="shared" si="0"/>
         <v>0.35416666666666663</v>
       </c>
-      <c r="C4" s="116">
+      <c r="C4" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A4,Journal[Temps])</f>
         <v>0.35416666666666663</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="114">
+      <c r="A5" s="132">
         <f/>
         <v>45974</v>
       </c>
-      <c r="B5" s="115">
+      <c r="B5" s="133">
         <f t="shared" si="0"/>
         <v>0.0625</v>
       </c>
-      <c r="C5" s="116">
+      <c r="C5" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A5,Journal[Temps])</f>
         <v>0.0625</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="114">
+      <c r="A6" s="132">
         <f/>
         <v>45979</v>
       </c>
-      <c r="B6" s="115">
+      <c r="B6" s="133">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C6" s="116">
+      <c r="C6" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A6,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="114">
+      <c r="A7" s="132">
         <f/>
         <v>45986</v>
       </c>
-      <c r="B7" s="115">
+      <c r="B7" s="133">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C7" s="116">
+      <c r="C7" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A7,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="114">
+      <c r="A8" s="132">
         <f/>
         <v>45993</v>
       </c>
-      <c r="B8" s="115">
+      <c r="B8" s="133">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C8" s="116">
+      <c r="C8" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A8,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="114">
+      <c r="A9" s="132">
         <f/>
         <v>45995</v>
       </c>
-      <c r="B9" s="115">
+      <c r="B9" s="133">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C9" s="116">
+      <c r="C9" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A9,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="114">
+      <c r="A10" s="132">
         <f/>
         <v>46000</v>
       </c>
-      <c r="B10" s="115">
+      <c r="B10" s="133">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C10" s="116">
+      <c r="C10" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A10,Journal[Temps])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="114">
+      <c r="A11" s="132">
         <f/>
         <v>46007</v>
       </c>
-      <c r="B11" s="115">
+      <c r="B11" s="133">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="C11" s="116">
+      <c r="C11" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A11,Journal[Temps])</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="114"/>
-      <c r="B12" s="115" t="str">
+      <c r="A12" s="132"/>
+      <c r="B12" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C12" s="116">
+      <c r="C12" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A12,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="114"/>
-      <c r="B13" s="115" t="str">
+      <c r="A13" s="132"/>
+      <c r="B13" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C13" s="116">
+      <c r="C13" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A13,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="114"/>
-      <c r="B14" s="115" t="str">
+      <c r="A14" s="132"/>
+      <c r="B14" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C14" s="116">
+      <c r="C14" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A14,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="114"/>
-      <c r="B15" s="115" t="str">
+      <c r="A15" s="132"/>
+      <c r="B15" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C15" s="116">
+      <c r="C15" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A15,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="114"/>
-      <c r="B16" s="115" t="str">
+      <c r="A16" s="132"/>
+      <c r="B16" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C16" s="116">
+      <c r="C16" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A16,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="114"/>
-      <c r="B17" s="115" t="str">
+      <c r="A17" s="132"/>
+      <c r="B17" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C17" s="116">
+      <c r="C17" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A17,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="114"/>
-      <c r="B18" s="115" t="str">
+      <c r="A18" s="132"/>
+      <c r="B18" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C18" s="116">
+      <c r="C18" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A18,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="114"/>
-      <c r="B19" s="115" t="str">
+      <c r="A19" s="132"/>
+      <c r="B19" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C19" s="116">
+      <c r="C19" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A19,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="114"/>
-      <c r="B20" s="115" t="str">
+      <c r="A20" s="132"/>
+      <c r="B20" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C20" s="116">
+      <c r="C20" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A20,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="114"/>
-      <c r="B21" s="115" t="str">
+      <c r="A21" s="132"/>
+      <c r="B21" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C21" s="116">
+      <c r="C21" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A21,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="114"/>
-      <c r="B22" s="115" t="str">
+      <c r="A22" s="132"/>
+      <c r="B22" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C22" s="116">
+      <c r="C22" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A22,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="114"/>
-      <c r="B23" s="115" t="str">
+      <c r="A23" s="132"/>
+      <c r="B23" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C23" s="116">
+      <c r="C23" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A23,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="114"/>
-      <c r="B24" s="115" t="str">
+      <c r="A24" s="132"/>
+      <c r="B24" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C24" s="116">
+      <c r="C24" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A24,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="114"/>
-      <c r="B25" s="115" t="str">
+      <c r="A25" s="132"/>
+      <c r="B25" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C25" s="116">
+      <c r="C25" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A25,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="114"/>
-      <c r="B26" s="115" t="str">
+      <c r="A26" s="132"/>
+      <c r="B26" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C26" s="116">
+      <c r="C26" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A26,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="114"/>
-      <c r="B27" s="115" t="str">
+      <c r="A27" s="132"/>
+      <c r="B27" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C27" s="116">
+      <c r="C27" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A27,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="114"/>
-      <c r="B28" s="115" t="str">
+      <c r="A28" s="132"/>
+      <c r="B28" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C28" s="116">
+      <c r="C28" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A28,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="114"/>
-      <c r="B29" s="115" t="str">
+      <c r="A29" s="132"/>
+      <c r="B29" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C29" s="116">
+      <c r="C29" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A29,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="114"/>
-      <c r="B30" s="115" t="str">
+      <c r="A30" s="132"/>
+      <c r="B30" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C30" s="116">
+      <c r="C30" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A30,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="114"/>
-      <c r="B31" s="115" t="str">
+      <c r="A31" s="132"/>
+      <c r="B31" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C31" s="116">
+      <c r="C31" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A31,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="114"/>
-      <c r="B32" s="115" t="str">
+      <c r="A32" s="132"/>
+      <c r="B32" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C32" s="116">
+      <c r="C32" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A32,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="114"/>
-      <c r="B33" s="115" t="str">
+      <c r="A33" s="132"/>
+      <c r="B33" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C33" s="116">
+      <c r="C33" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A33,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="114"/>
-      <c r="B34" s="115" t="str">
+      <c r="A34" s="132"/>
+      <c r="B34" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C34" s="116">
+      <c r="C34" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A34,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="114"/>
-      <c r="B35" s="115" t="str">
+      <c r="A35" s="132"/>
+      <c r="B35" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C35" s="116">
+      <c r="C35" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A35,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="114"/>
-      <c r="B36" s="115" t="str">
+      <c r="A36" s="132"/>
+      <c r="B36" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C36" s="116">
+      <c r="C36" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A36,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="114"/>
-      <c r="B37" s="115" t="str">
+      <c r="A37" s="132"/>
+      <c r="B37" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C37" s="116">
+      <c r="C37" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A37,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="114"/>
-      <c r="B38" s="115" t="str">
+      <c r="A38" s="132"/>
+      <c r="B38" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C38" s="116">
+      <c r="C38" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A38,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="117"/>
-      <c r="B39" s="115" t="str">
+      <c r="A39" s="135"/>
+      <c r="B39" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C39" s="116">
+      <c r="C39" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A39,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="117"/>
-      <c r="B40" s="115" t="str">
+      <c r="A40" s="135"/>
+      <c r="B40" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C40" s="116">
+      <c r="C40" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A40,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="117"/>
-      <c r="B41" s="115" t="str">
+      <c r="A41" s="135"/>
+      <c r="B41" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C41" s="116">
+      <c r="C41" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A41,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="117"/>
-      <c r="B42" s="115" t="str">
+      <c r="A42" s="135"/>
+      <c r="B42" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C42" s="116">
+      <c r="C42" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A42,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="117"/>
-      <c r="B43" s="115" t="str">
+      <c r="A43" s="135"/>
+      <c r="B43" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C43" s="116">
+      <c r="C43" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A43,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="117"/>
-      <c r="B44" s="115" t="str">
+      <c r="A44" s="135"/>
+      <c r="B44" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C44" s="116">
+      <c r="C44" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A44,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="117"/>
-      <c r="B45" s="115" t="str">
+      <c r="A45" s="135"/>
+      <c r="B45" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C45" s="116">
+      <c r="C45" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A45,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="117"/>
-      <c r="B46" s="115" t="str">
+      <c r="A46" s="135"/>
+      <c r="B46" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C46" s="116">
+      <c r="C46" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A46,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="117"/>
-      <c r="B47" s="115" t="str">
+      <c r="A47" s="135"/>
+      <c r="B47" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C47" s="116">
+      <c r="C47" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A47,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="117"/>
-      <c r="B48" s="115" t="str">
+      <c r="A48" s="135"/>
+      <c r="B48" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C48" s="116">
+      <c r="C48" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A48,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="117"/>
-      <c r="B49" s="115" t="str">
+      <c r="A49" s="135"/>
+      <c r="B49" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C49" s="116">
+      <c r="C49" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A49,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="117"/>
-      <c r="B50" s="115" t="str">
+      <c r="A50" s="135"/>
+      <c r="B50" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C50" s="116">
+      <c r="C50" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A50,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="117"/>
-      <c r="B51" s="115" t="str">
+      <c r="A51" s="135"/>
+      <c r="B51" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C51" s="116">
+      <c r="C51" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A51,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="117"/>
-      <c r="B52" s="115" t="str">
+      <c r="A52" s="135"/>
+      <c r="B52" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C52" s="116">
+      <c r="C52" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A52,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="117"/>
-      <c r="B53" s="115" t="str">
+      <c r="A53" s="135"/>
+      <c r="B53" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C53" s="116">
+      <c r="C53" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A53,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="117"/>
-      <c r="B54" s="115" t="str">
+      <c r="A54" s="135"/>
+      <c r="B54" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C54" s="116">
+      <c r="C54" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A54,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="117"/>
-      <c r="B55" s="115" t="str">
+      <c r="A55" s="135"/>
+      <c r="B55" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C55" s="116">
+      <c r="C55" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A55,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="117"/>
-      <c r="B56" s="115" t="str">
+      <c r="A56" s="135"/>
+      <c r="B56" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C56" s="116">
+      <c r="C56" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A56,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="117"/>
-      <c r="B57" s="115" t="str">
+      <c r="A57" s="135"/>
+      <c r="B57" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C57" s="116">
+      <c r="C57" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A57,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="117"/>
-      <c r="B58" s="115" t="str">
+      <c r="A58" s="135"/>
+      <c r="B58" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C58" s="116">
+      <c r="C58" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A58,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="117"/>
-      <c r="B59" s="115" t="str">
+      <c r="A59" s="135"/>
+      <c r="B59" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C59" s="116">
+      <c r="C59" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A59,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="117"/>
-      <c r="B60" s="115" t="str">
+      <c r="A60" s="135"/>
+      <c r="B60" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C60" s="116">
+      <c r="C60" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A60,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="117"/>
-      <c r="B61" s="115" t="str">
+      <c r="A61" s="135"/>
+      <c r="B61" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C61" s="116">
+      <c r="C61" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A61,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="117"/>
-      <c r="B62" s="115" t="str">
+      <c r="A62" s="135"/>
+      <c r="B62" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C62" s="116">
+      <c r="C62" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A62,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="117"/>
-      <c r="B63" s="115" t="str">
+      <c r="A63" s="135"/>
+      <c r="B63" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C63" s="116">
+      <c r="C63" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A63,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="117"/>
-      <c r="B64" s="115" t="str">
+      <c r="A64" s="135"/>
+      <c r="B64" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C64" s="116">
+      <c r="C64" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A64,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="117"/>
-      <c r="B65" s="115" t="str">
+      <c r="A65" s="135"/>
+      <c r="B65" s="133" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="C65" s="116">
+      <c r="C65" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A65,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="117"/>
-      <c r="B66" s="115" t="str">
+      <c r="A66" s="135"/>
+      <c r="B66" s="133" t="str">
         <f t="shared" ref="B66:B114" si="1">IF(C66&gt;0,C66,"")</f>
         <v/>
       </c>
-      <c r="C66" s="116">
+      <c r="C66" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A66,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="117"/>
-      <c r="B67" s="115" t="str">
+      <c r="A67" s="135"/>
+      <c r="B67" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C67" s="116">
+      <c r="C67" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A67,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="117"/>
-      <c r="B68" s="115" t="str">
+      <c r="A68" s="135"/>
+      <c r="B68" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C68" s="116">
+      <c r="C68" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A68,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="117"/>
-      <c r="B69" s="115" t="str">
+      <c r="A69" s="135"/>
+      <c r="B69" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C69" s="116">
+      <c r="C69" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A69,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="117"/>
-      <c r="B70" s="115" t="str">
+      <c r="A70" s="135"/>
+      <c r="B70" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C70" s="116">
+      <c r="C70" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A70,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="117"/>
-      <c r="B71" s="115" t="str">
+      <c r="A71" s="135"/>
+      <c r="B71" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C71" s="116">
+      <c r="C71" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A71,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="117"/>
-      <c r="B72" s="115" t="str">
+      <c r="A72" s="135"/>
+      <c r="B72" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C72" s="116">
+      <c r="C72" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A72,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="117"/>
-      <c r="B73" s="115" t="str">
+      <c r="A73" s="135"/>
+      <c r="B73" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C73" s="116">
+      <c r="C73" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A73,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="117"/>
-      <c r="B74" s="115" t="str">
+      <c r="A74" s="135"/>
+      <c r="B74" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C74" s="116">
+      <c r="C74" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A74,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="117"/>
-      <c r="B75" s="115" t="str">
+      <c r="A75" s="135"/>
+      <c r="B75" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C75" s="116">
+      <c r="C75" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A75,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="117"/>
-      <c r="B76" s="115" t="str">
+      <c r="A76" s="135"/>
+      <c r="B76" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C76" s="116">
+      <c r="C76" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A76,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="117"/>
-      <c r="B77" s="115" t="str">
+      <c r="A77" s="135"/>
+      <c r="B77" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C77" s="116">
+      <c r="C77" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A77,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="117"/>
-      <c r="B78" s="115" t="str">
+      <c r="A78" s="135"/>
+      <c r="B78" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C78" s="116">
+      <c r="C78" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A78,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="117"/>
-      <c r="B79" s="115" t="str">
+      <c r="A79" s="135"/>
+      <c r="B79" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C79" s="116">
+      <c r="C79" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A79,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="117"/>
-      <c r="B80" s="115" t="str">
+      <c r="A80" s="135"/>
+      <c r="B80" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C80" s="116">
+      <c r="C80" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A80,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="117"/>
-      <c r="B81" s="115" t="str">
+      <c r="A81" s="135"/>
+      <c r="B81" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C81" s="116">
+      <c r="C81" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A81,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="117"/>
-      <c r="B82" s="115" t="str">
+      <c r="A82" s="135"/>
+      <c r="B82" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C82" s="116">
+      <c r="C82" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A82,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="117"/>
-      <c r="B83" s="115" t="str">
+      <c r="A83" s="135"/>
+      <c r="B83" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C83" s="116">
+      <c r="C83" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A83,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="117"/>
-      <c r="B84" s="115" t="str">
+      <c r="A84" s="135"/>
+      <c r="B84" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C84" s="116">
+      <c r="C84" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A84,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="117"/>
-      <c r="B85" s="115" t="str">
+      <c r="A85" s="135"/>
+      <c r="B85" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C85" s="116">
+      <c r="C85" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A85,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="117"/>
-      <c r="B86" s="115" t="str">
+      <c r="A86" s="135"/>
+      <c r="B86" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C86" s="116">
+      <c r="C86" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A86,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="117"/>
-      <c r="B87" s="115" t="str">
+      <c r="A87" s="135"/>
+      <c r="B87" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C87" s="116">
+      <c r="C87" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A87,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="117"/>
-      <c r="B88" s="115" t="str">
+      <c r="A88" s="135"/>
+      <c r="B88" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C88" s="116">
+      <c r="C88" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A88,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="117"/>
-      <c r="B89" s="115" t="str">
+      <c r="A89" s="135"/>
+      <c r="B89" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C89" s="116">
+      <c r="C89" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A89,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="117"/>
-      <c r="B90" s="115" t="str">
+      <c r="A90" s="135"/>
+      <c r="B90" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C90" s="116">
+      <c r="C90" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A90,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="117"/>
-      <c r="B91" s="115" t="str">
+      <c r="A91" s="135"/>
+      <c r="B91" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C91" s="116">
+      <c r="C91" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A91,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="117"/>
-      <c r="B92" s="115" t="str">
+      <c r="A92" s="135"/>
+      <c r="B92" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C92" s="116">
+      <c r="C92" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A92,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="117"/>
-      <c r="B93" s="115" t="str">
+      <c r="A93" s="135"/>
+      <c r="B93" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C93" s="116">
+      <c r="C93" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A93,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="117"/>
-      <c r="B94" s="115" t="str">
+      <c r="A94" s="135"/>
+      <c r="B94" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C94" s="116">
+      <c r="C94" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A94,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="117"/>
-      <c r="B95" s="115" t="str">
+      <c r="A95" s="135"/>
+      <c r="B95" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C95" s="116">
+      <c r="C95" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A95,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="117"/>
-      <c r="B96" s="115" t="str">
+      <c r="A96" s="135"/>
+      <c r="B96" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C96" s="116">
+      <c r="C96" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A96,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="117"/>
-      <c r="B97" s="115" t="str">
+      <c r="A97" s="135"/>
+      <c r="B97" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C97" s="116">
+      <c r="C97" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A97,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="117"/>
-      <c r="B98" s="115" t="str">
+      <c r="A98" s="135"/>
+      <c r="B98" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C98" s="116">
+      <c r="C98" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A98,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="117"/>
-      <c r="B99" s="115" t="str">
+      <c r="A99" s="135"/>
+      <c r="B99" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C99" s="116">
+      <c r="C99" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A99,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="117"/>
-      <c r="B100" s="115" t="str">
+      <c r="A100" s="135"/>
+      <c r="B100" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C100" s="116">
+      <c r="C100" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A100,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="117"/>
-      <c r="B101" s="115" t="str">
+      <c r="A101" s="135"/>
+      <c r="B101" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C101" s="116">
+      <c r="C101" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A101,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="117"/>
-      <c r="B102" s="115" t="str">
+      <c r="A102" s="135"/>
+      <c r="B102" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C102" s="116">
+      <c r="C102" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A102,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="117"/>
-      <c r="B103" s="115" t="str">
+      <c r="A103" s="135"/>
+      <c r="B103" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C103" s="116">
+      <c r="C103" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A103,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="117"/>
-      <c r="B104" s="115" t="str">
+      <c r="A104" s="135"/>
+      <c r="B104" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C104" s="116">
+      <c r="C104" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A104,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="117"/>
-      <c r="B105" s="115" t="str">
+      <c r="A105" s="135"/>
+      <c r="B105" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C105" s="116">
+      <c r="C105" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A105,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="117"/>
-      <c r="B106" s="115" t="str">
+      <c r="A106" s="135"/>
+      <c r="B106" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C106" s="116">
+      <c r="C106" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A106,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="117"/>
-      <c r="B107" s="115" t="str">
+      <c r="A107" s="135"/>
+      <c r="B107" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C107" s="116">
+      <c r="C107" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A107,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="117"/>
-      <c r="B108" s="115" t="str">
+      <c r="A108" s="135"/>
+      <c r="B108" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C108" s="116">
+      <c r="C108" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A108,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="117"/>
-      <c r="B109" s="115" t="str">
+      <c r="A109" s="135"/>
+      <c r="B109" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C109" s="116">
+      <c r="C109" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A109,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="117"/>
-      <c r="B110" s="115" t="str">
+      <c r="A110" s="135"/>
+      <c r="B110" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C110" s="116">
+      <c r="C110" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A110,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="117"/>
-      <c r="B111" s="115" t="str">
+      <c r="A111" s="135"/>
+      <c r="B111" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C111" s="116">
+      <c r="C111" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A111,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="117"/>
-      <c r="B112" s="115" t="str">
+      <c r="A112" s="135"/>
+      <c r="B112" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C112" s="116">
+      <c r="C112" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A112,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="117"/>
-      <c r="B113" s="115" t="str">
+      <c r="A113" s="135"/>
+      <c r="B113" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C113" s="116">
+      <c r="C113" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A113,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="117"/>
-      <c r="B114" s="115" t="str">
+      <c r="A114" s="135"/>
+      <c r="B114" s="133" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="C114" s="116">
+      <c r="C114" s="134">
         <f>SUMIF(Journal[date],SommeParJours!A114,Journal[Temps])</f>
         <v>0</v>
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="117"/>
-      <c r="B115" s="117"/>
-      <c r="C115" s="116"/>
+      <c r="A115" s="135"/>
+      <c r="B115" s="135"/>
+      <c r="C115" s="134"/>
     </row>
     <row r="116">
-      <c r="A116" s="117"/>
-      <c r="B116" s="117"/>
-      <c r="C116" s="116"/>
+      <c r="A116" s="135"/>
+      <c r="B116" s="135"/>
+      <c r="C116" s="134"/>
     </row>
     <row r="117">
-      <c r="A117" s="117"/>
-      <c r="B117" s="117"/>
-      <c r="C117" s="116"/>
+      <c r="A117" s="135"/>
+      <c r="B117" s="135"/>
+      <c r="C117" s="134"/>
     </row>
     <row r="118">
-      <c r="A118" s="117"/>
-      <c r="B118" s="117"/>
-      <c r="C118" s="116"/>
+      <c r="A118" s="135"/>
+      <c r="B118" s="135"/>
+      <c r="C118" s="134"/>
     </row>
     <row r="119">
-      <c r="A119" s="117"/>
-      <c r="B119" s="117"/>
-      <c r="C119" s="116"/>
+      <c r="A119" s="135"/>
+      <c r="B119" s="135"/>
+      <c r="C119" s="134"/>
     </row>
     <row r="120">
-      <c r="A120" s="117"/>
-      <c r="B120" s="117"/>
-      <c r="C120" s="116"/>
+      <c r="A120" s="135"/>
+      <c r="B120" s="135"/>
+      <c r="C120" s="134"/>
     </row>
     <row r="121">
-      <c r="A121" s="117"/>
-      <c r="B121" s="117"/>
-      <c r="C121" s="116"/>
+      <c r="A121" s="135"/>
+      <c r="B121" s="135"/>
+      <c r="C121" s="134"/>
     </row>
     <row r="122">
-      <c r="A122" s="117"/>
-      <c r="B122" s="117"/>
-      <c r="C122" s="116"/>
+      <c r="A122" s="135"/>
+      <c r="B122" s="135"/>
+      <c r="C122" s="134"/>
     </row>
     <row r="123">
-      <c r="A123" s="117"/>
-      <c r="B123" s="117"/>
-      <c r="C123" s="116"/>
+      <c r="A123" s="135"/>
+      <c r="B123" s="135"/>
+      <c r="C123" s="134"/>
     </row>
     <row r="124">
-      <c r="A124" s="117"/>
-      <c r="B124" s="117"/>
-      <c r="C124" s="116"/>
+      <c r="A124" s="135"/>
+      <c r="B124" s="135"/>
+      <c r="C124" s="134"/>
     </row>
     <row r="125">
-      <c r="A125" s="117"/>
-      <c r="B125" s="117"/>
-      <c r="C125" s="116"/>
+      <c r="A125" s="135"/>
+      <c r="B125" s="135"/>
+      <c r="C125" s="134"/>
     </row>
     <row r="126">
-      <c r="A126" s="117"/>
-      <c r="B126" s="117"/>
-      <c r="C126" s="116"/>
+      <c r="A126" s="135"/>
+      <c r="B126" s="135"/>
+      <c r="C126" s="134"/>
     </row>
     <row r="127">
-      <c r="A127" s="117"/>
-      <c r="B127" s="117"/>
-      <c r="C127" s="116"/>
+      <c r="A127" s="135"/>
+      <c r="B127" s="135"/>
+      <c r="C127" s="134"/>
     </row>
     <row r="128">
-      <c r="A128" s="117"/>
-      <c r="B128" s="117"/>
-      <c r="C128" s="116"/>
+      <c r="A128" s="135"/>
+      <c r="B128" s="135"/>
+      <c r="C128" s="134"/>
     </row>
     <row r="129">
-      <c r="A129" s="117"/>
-      <c r="B129" s="117"/>
-      <c r="C129" s="116"/>
+      <c r="A129" s="135"/>
+      <c r="B129" s="135"/>
+      <c r="C129" s="134"/>
     </row>
     <row r="130">
-      <c r="A130" s="117"/>
-      <c r="B130" s="117"/>
-      <c r="C130" s="116"/>
+      <c r="A130" s="135"/>
+      <c r="B130" s="135"/>
+      <c r="C130" s="134"/>
     </row>
     <row r="131">
-      <c r="A131" s="117"/>
-      <c r="B131" s="117"/>
-      <c r="C131" s="116"/>
+      <c r="A131" s="135"/>
+      <c r="B131" s="135"/>
+      <c r="C131" s="134"/>
     </row>
     <row r="132">
-      <c r="A132" s="117"/>
-      <c r="B132" s="117"/>
-      <c r="C132" s="116"/>
+      <c r="A132" s="135"/>
+      <c r="B132" s="135"/>
+      <c r="C132" s="134"/>
     </row>
     <row r="133">
-      <c r="A133" s="117"/>
-      <c r="B133" s="117"/>
-      <c r="C133" s="116"/>
+      <c r="A133" s="135"/>
+      <c r="B133" s="135"/>
+      <c r="C133" s="134"/>
     </row>
     <row r="134">
-      <c r="A134" s="117"/>
-      <c r="B134" s="117"/>
-      <c r="C134" s="116"/>
+      <c r="A134" s="135"/>
+      <c r="B134" s="135"/>
+      <c r="C134" s="134"/>
     </row>
     <row r="135">
-      <c r="A135" s="117"/>
-      <c r="B135" s="117"/>
-      <c r="C135" s="116"/>
+      <c r="A135" s="135"/>
+      <c r="B135" s="135"/>
+      <c r="C135" s="134"/>
     </row>
     <row r="136">
-      <c r="A136" s="117"/>
-      <c r="B136" s="117"/>
-      <c r="C136" s="116"/>
+      <c r="A136" s="135"/>
+      <c r="B136" s="135"/>
+      <c r="C136" s="134"/>
     </row>
     <row r="137">
-      <c r="A137" s="117"/>
-      <c r="B137" s="117"/>
-      <c r="C137" s="116"/>
+      <c r="A137" s="135"/>
+      <c r="B137" s="135"/>
+      <c r="C137" s="134"/>
     </row>
     <row r="138">
-      <c r="A138" s="117"/>
-      <c r="B138" s="117"/>
-      <c r="C138" s="116"/>
+      <c r="A138" s="135"/>
+      <c r="B138" s="135"/>
+      <c r="C138" s="134"/>
     </row>
     <row r="139">
-      <c r="A139" s="117"/>
-      <c r="B139" s="117"/>
-      <c r="C139" s="116"/>
+      <c r="A139" s="135"/>
+      <c r="B139" s="135"/>
+      <c r="C139" s="134"/>
     </row>
     <row r="140">
-      <c r="A140" s="117"/>
-      <c r="B140" s="117"/>
-      <c r="C140" s="116"/>
+      <c r="A140" s="135"/>
+      <c r="B140" s="135"/>
+      <c r="C140" s="134"/>
     </row>
     <row r="141">
-      <c r="A141" s="117"/>
-      <c r="B141" s="117"/>
-      <c r="C141" s="116"/>
+      <c r="A141" s="135"/>
+      <c r="B141" s="135"/>
+      <c r="C141" s="134"/>
     </row>
     <row r="142">
-      <c r="A142" s="117"/>
-      <c r="B142" s="117"/>
-      <c r="C142" s="116"/>
+      <c r="A142" s="135"/>
+      <c r="B142" s="135"/>
+      <c r="C142" s="134"/>
     </row>
     <row r="143">
-      <c r="A143" s="117"/>
-      <c r="B143" s="117"/>
-      <c r="C143" s="116"/>
+      <c r="A143" s="135"/>
+      <c r="B143" s="135"/>
+      <c r="C143" s="134"/>
     </row>
     <row r="144">
-      <c r="A144" s="117"/>
-      <c r="B144" s="117"/>
-      <c r="C144" s="116"/>
+      <c r="A144" s="135"/>
+      <c r="B144" s="135"/>
+      <c r="C144" s="134"/>
     </row>
     <row r="145">
-      <c r="A145" s="117"/>
-      <c r="B145" s="117"/>
-      <c r="C145" s="116"/>
+      <c r="A145" s="135"/>
+      <c r="B145" s="135"/>
+      <c r="C145" s="134"/>
     </row>
     <row r="146">
-      <c r="A146" s="117"/>
-      <c r="B146" s="117"/>
-      <c r="C146" s="116"/>
+      <c r="A146" s="135"/>
+      <c r="B146" s="135"/>
+      <c r="C146" s="134"/>
     </row>
     <row r="147">
-      <c r="A147" s="117"/>
-      <c r="B147" s="117"/>
-      <c r="C147" s="116"/>
+      <c r="A147" s="135"/>
+      <c r="B147" s="135"/>
+      <c r="C147" s="134"/>
     </row>
     <row r="148">
-      <c r="A148" s="117"/>
-      <c r="B148" s="117"/>
-      <c r="C148" s="116"/>
+      <c r="A148" s="135"/>
+      <c r="B148" s="135"/>
+      <c r="C148" s="134"/>
     </row>
     <row r="149">
-      <c r="A149" s="117"/>
-      <c r="B149" s="117"/>
-      <c r="C149" s="116"/>
+      <c r="A149" s="135"/>
+      <c r="B149" s="135"/>
+      <c r="C149" s="134"/>
     </row>
     <row r="150">
-      <c r="A150" s="117"/>
-      <c r="B150" s="117"/>
-      <c r="C150" s="116"/>
+      <c r="A150" s="135"/>
+      <c r="B150" s="135"/>
+      <c r="C150" s="134"/>
     </row>
     <row r="151">
-      <c r="A151" s="117"/>
-      <c r="B151" s="117"/>
-      <c r="C151" s="116"/>
+      <c r="A151" s="135"/>
+      <c r="B151" s="135"/>
+      <c r="C151" s="134"/>
     </row>
     <row r="152">
-      <c r="A152" s="117"/>
-      <c r="B152" s="117"/>
-      <c r="C152" s="116"/>
+      <c r="A152" s="135"/>
+      <c r="B152" s="135"/>
+      <c r="C152" s="134"/>
     </row>
     <row r="153">
-      <c r="A153" s="117"/>
-      <c r="B153" s="117"/>
-      <c r="C153" s="116"/>
+      <c r="A153" s="135"/>
+      <c r="B153" s="135"/>
+      <c r="C153" s="134"/>
     </row>
     <row r="154">
-      <c r="A154" s="117"/>
-      <c r="B154" s="117"/>
-      <c r="C154" s="116"/>
+      <c r="A154" s="135"/>
+      <c r="B154" s="135"/>
+      <c r="C154" s="134"/>
     </row>
     <row r="155">
-      <c r="A155" s="117"/>
-      <c r="B155" s="117"/>
-      <c r="C155" s="116"/>
+      <c r="A155" s="135"/>
+      <c r="B155" s="135"/>
+      <c r="C155" s="134"/>
     </row>
     <row r="156">
-      <c r="A156" s="117"/>
-      <c r="B156" s="117"/>
-      <c r="C156" s="116"/>
+      <c r="A156" s="135"/>
+      <c r="B156" s="135"/>
+      <c r="C156" s="134"/>
     </row>
     <row r="157">
-      <c r="A157" s="117"/>
-      <c r="B157" s="117"/>
-      <c r="C157" s="116"/>
+      <c r="A157" s="135"/>
+      <c r="B157" s="135"/>
+      <c r="C157" s="134"/>
     </row>
     <row r="158">
-      <c r="A158" s="117"/>
-      <c r="B158" s="117"/>
-      <c r="C158" s="116"/>
+      <c r="A158" s="135"/>
+      <c r="B158" s="135"/>
+      <c r="C158" s="134"/>
     </row>
     <row r="159">
-      <c r="A159" s="117"/>
-      <c r="B159" s="117"/>
+      <c r="A159" s="135"/>
+      <c r="B159" s="135"/>
     </row>
     <row r="160">
-      <c r="A160" s="117"/>
-      <c r="B160" s="117"/>
+      <c r="A160" s="135"/>
+      <c r="B160" s="135"/>
     </row>
     <row r="161">
-      <c r="A161" s="117"/>
-      <c r="B161" s="117"/>
+      <c r="A161" s="135"/>
+      <c r="B161" s="135"/>
     </row>
     <row r="162">
-      <c r="A162" s="117"/>
-      <c r="B162" s="117"/>
+      <c r="A162" s="135"/>
+      <c r="B162" s="135"/>
     </row>
     <row r="163">
-      <c r="A163" s="117"/>
-      <c r="B163" s="117"/>
+      <c r="A163" s="135"/>
+      <c r="B163" s="135"/>
     </row>
     <row r="164">
-      <c r="A164" s="117"/>
-      <c r="B164" s="117"/>
+      <c r="A164" s="135"/>
+      <c r="B164" s="135"/>
     </row>
     <row r="165">
-      <c r="A165" s="117"/>
-      <c r="B165" s="117"/>
+      <c r="A165" s="135"/>
+      <c r="B165" s="135"/>
     </row>
     <row r="166">
-      <c r="A166" s="117"/>
-      <c r="B166" s="117"/>
+      <c r="A166" s="135"/>
+      <c r="B166" s="135"/>
     </row>
     <row r="167">
-      <c r="A167" s="117"/>
-      <c r="B167" s="117"/>
+      <c r="A167" s="135"/>
+      <c r="B167" s="135"/>
     </row>
     <row r="168">
-      <c r="A168" s="117"/>
-      <c r="B168" s="117"/>
+      <c r="A168" s="135"/>
+      <c r="B168" s="135"/>
     </row>
     <row r="169">
-      <c r="A169" s="117"/>
-      <c r="B169" s="117"/>
+      <c r="A169" s="135"/>
+      <c r="B169" s="135"/>
     </row>
     <row r="170">
-      <c r="A170" s="117"/>
-      <c r="B170" s="117"/>
+      <c r="A170" s="135"/>
+      <c r="B170" s="135"/>
     </row>
     <row r="171">
-      <c r="A171" s="117"/>
-      <c r="B171" s="117"/>
+      <c r="A171" s="135"/>
+      <c r="B171" s="135"/>
     </row>
     <row r="172">
-      <c r="A172" s="117"/>
-      <c r="B172" s="117"/>
+      <c r="A172" s="135"/>
+      <c r="B172" s="135"/>
     </row>
     <row r="173">
-      <c r="A173" s="117"/>
-      <c r="B173" s="117"/>
+      <c r="A173" s="135"/>
+      <c r="B173" s="135"/>
     </row>
     <row r="174">
-      <c r="A174" s="117"/>
-      <c r="B174" s="117"/>
+      <c r="A174" s="135"/>
+      <c r="B174" s="135"/>
     </row>
     <row r="175">
-      <c r="A175" s="117"/>
-      <c r="B175" s="117"/>
+      <c r="A175" s="135"/>
+      <c r="B175" s="135"/>
     </row>
     <row r="176">
-      <c r="A176" s="117"/>
-      <c r="B176" s="117"/>
+      <c r="A176" s="135"/>
+      <c r="B176" s="135"/>
     </row>
     <row r="177">
-      <c r="A177" s="117"/>
-      <c r="B177" s="117"/>
+      <c r="A177" s="135"/>
+      <c r="B177" s="135"/>
     </row>
     <row r="178">
-      <c r="A178" s="117"/>
-      <c r="B178" s="117"/>
+      <c r="A178" s="135"/>
+      <c r="B178" s="135"/>
     </row>
     <row r="179">
-      <c r="A179" s="117"/>
-      <c r="B179" s="117"/>
+      <c r="A179" s="135"/>
+      <c r="B179" s="135"/>
     </row>
     <row r="180">
-      <c r="A180" s="117"/>
-      <c r="B180" s="117"/>
+      <c r="A180" s="135"/>
+      <c r="B180" s="135"/>
     </row>
     <row r="181">
-      <c r="A181" s="117"/>
-      <c r="B181" s="117"/>
+      <c r="A181" s="135"/>
+      <c r="B181" s="135"/>
     </row>
     <row r="182">
-      <c r="A182" s="117"/>
-      <c r="B182" s="117"/>
+      <c r="A182" s="135"/>
+      <c r="B182" s="135"/>
     </row>
     <row r="183">
-      <c r="A183" s="117"/>
-      <c r="B183" s="117"/>
+      <c r="A183" s="135"/>
+      <c r="B183" s="135"/>
     </row>
     <row r="184">
-      <c r="A184" s="117"/>
-      <c r="B184" s="117"/>
+      <c r="A184" s="135"/>
+      <c r="B184" s="135"/>
     </row>
     <row r="185">
-      <c r="A185" s="117"/>
-      <c r="B185" s="117"/>
+      <c r="A185" s="135"/>
+      <c r="B185" s="135"/>
     </row>
     <row r="186">
-      <c r="A186" s="117"/>
-      <c r="B186" s="117"/>
+      <c r="A186" s="135"/>
+      <c r="B186" s="135"/>
     </row>
     <row r="187">
-      <c r="A187" s="117"/>
-      <c r="B187" s="117"/>
+      <c r="A187" s="135"/>
+      <c r="B187" s="135"/>
     </row>
     <row r="188">
-      <c r="A188" s="117"/>
-      <c r="B188" s="117"/>
+      <c r="A188" s="135"/>
+      <c r="B188" s="135"/>
     </row>
     <row r="189">
-      <c r="A189" s="117"/>
-      <c r="B189" s="117"/>
+      <c r="A189" s="135"/>
+      <c r="B189" s="135"/>
     </row>
     <row r="190">
-      <c r="A190" s="117"/>
-      <c r="B190" s="117"/>
+      <c r="A190" s="135"/>
+      <c r="B190" s="135"/>
     </row>
     <row r="191">
-      <c r="A191" s="117"/>
-      <c r="B191" s="117"/>
+      <c r="A191" s="135"/>
+      <c r="B191" s="135"/>
     </row>
     <row r="192">
-      <c r="A192" s="117"/>
-      <c r="B192" s="117"/>
+      <c r="A192" s="135"/>
+      <c r="B192" s="135"/>
     </row>
     <row r="193">
-      <c r="A193" s="117"/>
-      <c r="B193" s="117"/>
+      <c r="A193" s="135"/>
+      <c r="B193" s="135"/>
     </row>
     <row r="194">
-      <c r="A194" s="117"/>
-      <c r="B194" s="117"/>
+      <c r="A194" s="135"/>
+      <c r="B194" s="135"/>
     </row>
     <row r="195">
-      <c r="A195" s="117"/>
-      <c r="B195" s="117"/>
+      <c r="A195" s="135"/>
+      <c r="B195" s="135"/>
     </row>
     <row r="196">
-      <c r="A196" s="117"/>
-      <c r="B196" s="117"/>
+      <c r="A196" s="135"/>
+      <c r="B196" s="135"/>
     </row>
     <row r="197">
-      <c r="A197" s="117"/>
-      <c r="B197" s="117"/>
+      <c r="A197" s="135"/>
+      <c r="B197" s="135"/>
     </row>
     <row r="198">
-      <c r="A198" s="117"/>
-      <c r="B198" s="117"/>
+      <c r="A198" s="135"/>
+      <c r="B198" s="135"/>
     </row>
     <row r="199">
-      <c r="A199" s="117"/>
-      <c r="B199" s="117"/>
+      <c r="A199" s="135"/>
+      <c r="B199" s="135"/>
     </row>
     <row r="200">
-      <c r="A200" s="117"/>
-      <c r="B200" s="117"/>
+      <c r="A200" s="135"/>
+      <c r="B200" s="135"/>
     </row>
     <row r="201">
-      <c r="A201" s="117"/>
-      <c r="B201" s="117"/>
+      <c r="A201" s="135"/>
+      <c r="B201" s="135"/>
     </row>
     <row r="202">
-      <c r="A202" s="117"/>
-      <c r="B202" s="117"/>
+      <c r="A202" s="135"/>
+      <c r="B202" s="135"/>
     </row>
     <row r="203">
-      <c r="A203" s="117"/>
-      <c r="B203" s="117"/>
+      <c r="A203" s="135"/>
+      <c r="B203" s="135"/>
     </row>
     <row r="204">
-      <c r="A204" s="117"/>
-      <c r="B204" s="117"/>
+      <c r="A204" s="135"/>
+      <c r="B204" s="135"/>
     </row>
     <row r="205">
-      <c r="A205" s="117"/>
-      <c r="B205" s="117"/>
+      <c r="A205" s="135"/>
+      <c r="B205" s="135"/>
     </row>
     <row r="206">
-      <c r="A206" s="117"/>
-      <c r="B206" s="117"/>
+      <c r="A206" s="135"/>
+      <c r="B206" s="135"/>
     </row>
     <row r="207">
-      <c r="A207" s="117"/>
-      <c r="B207" s="117"/>
+      <c r="A207" s="135"/>
+      <c r="B207" s="135"/>
     </row>
     <row r="208">
-      <c r="A208" s="117"/>
-      <c r="B208" s="117"/>
+      <c r="A208" s="135"/>
+      <c r="B208" s="135"/>
     </row>
     <row r="209">
-      <c r="A209" s="117"/>
-      <c r="B209" s="117"/>
+      <c r="A209" s="135"/>
+      <c r="B209" s="135"/>
     </row>
     <row r="210">
-      <c r="A210" s="117"/>
-      <c r="B210" s="117"/>
+      <c r="A210" s="135"/>
+      <c r="B210" s="135"/>
     </row>
     <row r="211">
-      <c r="A211" s="117"/>
-      <c r="B211" s="117"/>
+      <c r="A211" s="135"/>
+      <c r="B211" s="135"/>
     </row>
     <row r="212">
-      <c r="A212" s="117"/>
-      <c r="B212" s="117"/>
+      <c r="A212" s="135"/>
+      <c r="B212" s="135"/>
     </row>
     <row r="213">
-      <c r="A213" s="117"/>
-      <c r="B213" s="117"/>
+      <c r="A213" s="135"/>
+      <c r="B213" s="135"/>
     </row>
     <row r="214">
-      <c r="A214" s="117"/>
-      <c r="B214" s="117"/>
+      <c r="A214" s="135"/>
+      <c r="B214" s="135"/>
     </row>
     <row r="215">
-      <c r="A215" s="117"/>
-      <c r="B215" s="117"/>
+      <c r="A215" s="135"/>
+      <c r="B215" s="135"/>
     </row>
     <row r="216">
-      <c r="A216" s="117"/>
-      <c r="B216" s="117"/>
+      <c r="A216" s="135"/>
+      <c r="B216" s="135"/>
     </row>
     <row r="217">
-      <c r="A217" s="117"/>
-      <c r="B217" s="117"/>
+      <c r="A217" s="135"/>
+      <c r="B217" s="135"/>
     </row>
     <row r="218">
-      <c r="A218" s="117"/>
-      <c r="B218" s="117"/>
+      <c r="A218" s="135"/>
+      <c r="B218" s="135"/>
     </row>
     <row r="219">
-      <c r="A219" s="117"/>
-      <c r="B219" s="117"/>
+      <c r="A219" s="135"/>
+      <c r="B219" s="135"/>
     </row>
     <row r="220">
-      <c r="A220" s="117"/>
-      <c r="B220" s="117"/>
+      <c r="A220" s="135"/>
+      <c r="B220" s="135"/>
     </row>
     <row r="221">
-      <c r="A221" s="117"/>
-      <c r="B221" s="117"/>
+      <c r="A221" s="135"/>
+      <c r="B221" s="135"/>
     </row>
     <row r="222">
-      <c r="A222" s="117"/>
-      <c r="B222" s="117"/>
+      <c r="A222" s="135"/>
+      <c r="B222" s="135"/>
     </row>
     <row r="223">
-      <c r="A223" s="117"/>
-      <c r="B223" s="117"/>
+      <c r="A223" s="135"/>
+      <c r="B223" s="135"/>
     </row>
     <row r="224">
-      <c r="A224" s="117"/>
-      <c r="B224" s="117"/>
+      <c r="A224" s="135"/>
+      <c r="B224" s="135"/>
     </row>
     <row r="225">
-      <c r="A225" s="117"/>
-      <c r="B225" s="117"/>
+      <c r="A225" s="135"/>
+      <c r="B225" s="135"/>
     </row>
     <row r="226">
-      <c r="A226" s="117"/>
-      <c r="B226" s="117"/>
+      <c r="A226" s="135"/>
+      <c r="B226" s="135"/>
     </row>
     <row r="227">
-      <c r="A227" s="117"/>
-      <c r="B227" s="117"/>
+      <c r="A227" s="135"/>
+      <c r="B227" s="135"/>
     </row>
     <row r="228">
-      <c r="A228" s="117"/>
-      <c r="B228" s="117"/>
+      <c r="A228" s="135"/>
+      <c r="B228" s="135"/>
     </row>
     <row r="229">
-      <c r="A229" s="117"/>
-      <c r="B229" s="117"/>
+      <c r="A229" s="135"/>
+      <c r="B229" s="135"/>
     </row>
     <row r="230">
-      <c r="A230" s="117"/>
-      <c r="B230" s="117"/>
+      <c r="A230" s="135"/>
+      <c r="B230" s="135"/>
     </row>
     <row r="231">
-      <c r="A231" s="117"/>
-      <c r="B231" s="117"/>
+      <c r="A231" s="135"/>
+      <c r="B231" s="135"/>
     </row>
     <row r="232">
-      <c r="A232" s="117"/>
-      <c r="B232" s="117"/>
+      <c r="A232" s="135"/>
+      <c r="B232" s="135"/>
     </row>
     <row r="233">
-      <c r="A233" s="117"/>
-      <c r="B233" s="117"/>
+      <c r="A233" s="135"/>
+      <c r="B233" s="135"/>
     </row>
     <row r="234">
-      <c r="A234" s="117"/>
-      <c r="B234" s="117"/>
+      <c r="A234" s="135"/>
+      <c r="B234" s="135"/>
     </row>
     <row r="235">
-      <c r="A235" s="117"/>
-      <c r="B235" s="117"/>
+      <c r="A235" s="135"/>
+      <c r="B235" s="135"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>